<commit_message>
Updated Test Cases XML file with comments. Removed Old Non-Working proj
</commit_message>
<xml_diff>
--- a/Tests/CS3202 Test Cases.xlsx
+++ b/Tests/CS3202 Test Cases.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saima Mahmood\Documents\NUS\Sem 6\CS3201_CS3202 Software Engineering\cs3202 team 4 repo\Tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t>Test Queries</t>
   </si>
@@ -22,9 +30,6 @@
     <t>Purpose of Test Case</t>
   </si>
   <si>
-    <t>4/10 - Status</t>
-  </si>
-  <si>
     <t>Queries1_TestBasic</t>
   </si>
   <si>
@@ -211,7 +216,7 @@
     <t>Source3</t>
   </si>
   <si>
-    <t>Pattern and Suchthat </t>
+    <t>Pattern and Suchthat</t>
   </si>
   <si>
     <t>TestPatternandSuchthat_Query4</t>
@@ -220,7 +225,7 @@
     <t>Source4</t>
   </si>
   <si>
-    <t>Pattern and Suchthat </t>
+    <t>Pattern and Suchthat</t>
   </si>
   <si>
     <t>TestBasicFollowsFollowsStar_Query6</t>
@@ -344,29 +349,52 @@
   </si>
   <si>
     <t>Source10</t>
+  </si>
+  <si>
+    <t>Query 12 &amp; 10: Patt is on the wrong side</t>
+  </si>
+  <si>
+    <t>4/10 - Status (Querys with incorrect results mentioned)</t>
+  </si>
+  <si>
+    <t>Query 8: Patt is on the wrong side,  Query 9: Autotester stops working, need to handle invalid query case</t>
+  </si>
+  <si>
+    <t>Query 9: outputs 4 and not 5 (smth wrong with the w stmt)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Query 2: Autotester stops working </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only tested till source 6 so far. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FF366092"/>
+      <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="3">
@@ -386,469 +414,752 @@
       <bottom style="thin">
         <color rgb="FF1C4587"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
-      <alignment/>
-    </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="2" applyFont="1" fontId="2">
-      <alignment/>
-    </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="2" applyFont="1" fontId="2">
-      <alignment/>
-    </xf>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" customWidth="1" max="1" width="42.0"/>
-    <col min="2" customWidth="1" max="2" width="29.29"/>
-    <col min="3" customWidth="1" max="3" width="44.29"/>
+    <col min="1" max="1" width="42" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" customWidth="1"/>
+    <col min="4" max="4" width="46.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="1" r="B1">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c t="s" s="1" r="C1">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="1" r="D1">
+      <c r="D1" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2">
-      <c t="s" s="2" r="A2">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c t="s" s="2" r="B2">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c t="s" s="3" r="C2">
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3">
-      <c t="s" s="3" r="A3">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="3" r="B3">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c t="s" s="3" r="C3">
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4">
-      <c t="s" s="3" r="A4">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c t="s" s="3" r="B4">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="3" r="C4">
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5">
-      <c t="s" s="3" r="A5">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c t="s" s="3" r="B5">
+      <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c t="s" s="3" r="C5">
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6">
-      <c t="s" s="3" r="A6">
+      <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
-      <c t="s" s="3" r="B6">
+      <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="3" r="C6">
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7">
-      <c t="s" s="3" r="A7">
+      <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
-      <c t="s" s="3" r="B7">
+      <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
-      <c t="s" s="3" r="C7">
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8">
-      <c t="s" s="3" r="A8">
+      <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
-      <c t="s" s="3" r="B8">
+      <c r="C8" s="3" t="s">
         <v>23</v>
       </c>
-      <c t="s" s="3" r="C8">
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9">
-      <c t="s" s="3" r="A9">
+      <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="3" r="B9">
+      <c r="C9" s="3" t="s">
         <v>26</v>
       </c>
-      <c t="s" s="3" r="C9">
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10">
-      <c t="s" s="3" r="A10">
+      <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
-      <c t="s" s="3" r="B10">
+      <c r="C10" s="3" t="s">
         <v>29</v>
       </c>
-      <c t="s" s="3" r="C10">
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11">
-      <c t="s" s="3" r="A11">
+      <c r="B11" s="3" t="s">
         <v>31</v>
       </c>
-      <c t="s" s="3" r="B11">
+      <c r="C11" s="3" t="s">
         <v>32</v>
       </c>
-      <c t="s" s="3" r="C11">
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12">
-      <c t="s" s="3" r="A12">
+      <c r="B12" s="3" t="s">
         <v>34</v>
       </c>
-      <c t="s" s="3" r="B12">
+      <c r="C12" s="3" t="s">
         <v>35</v>
       </c>
-      <c t="s" s="3" r="C12">
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13">
-      <c t="s" s="3" r="A13">
+      <c r="B13" s="3" t="s">
         <v>37</v>
       </c>
-      <c t="s" s="3" r="B13">
+      <c r="C13" s="3" t="s">
         <v>38</v>
       </c>
-      <c t="s" s="3" r="C13">
+    </row>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14">
-      <c t="s" s="3" r="A14">
+      <c r="B14" s="3" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="3" r="B14">
+      <c r="C14" s="3" t="s">
         <v>41</v>
       </c>
-      <c t="s" s="3" r="C14">
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="15">
-      <c t="s" s="3" r="A15">
+      <c r="B15" s="3" t="s">
         <v>43</v>
       </c>
-      <c t="s" s="3" r="B15">
+      <c r="C15" s="3" t="s">
         <v>44</v>
       </c>
-      <c t="s" s="3" r="C15">
+    </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16">
-      <c t="s" s="3" r="A16">
+      <c r="B16" s="3" t="s">
         <v>46</v>
       </c>
-      <c t="s" s="3" r="B16">
+      <c r="C16" s="3" t="s">
         <v>47</v>
       </c>
-      <c t="s" s="3" r="C16">
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17">
-      <c t="s" s="3" r="A17">
+      <c r="B17" s="3" t="s">
         <v>49</v>
       </c>
-      <c t="s" s="3" r="B17">
+      <c r="C17" s="3" t="s">
         <v>50</v>
       </c>
-      <c t="s" s="3" r="C17">
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18">
-      <c t="s" s="3" r="A18">
+      <c r="B18" s="3" t="s">
         <v>52</v>
       </c>
-      <c t="s" s="3" r="B18">
+      <c r="C18" s="3" t="s">
         <v>53</v>
       </c>
-      <c t="s" s="3" r="C18">
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19">
-      <c t="s" s="3" r="A19">
+      <c r="B19" s="3" t="s">
         <v>55</v>
       </c>
-      <c t="s" s="3" r="B19">
+      <c r="C19" s="3" t="s">
         <v>56</v>
       </c>
-      <c t="s" s="3" r="C19">
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="20">
-      <c t="s" s="3" r="A20">
+      <c r="B20" s="3" t="s">
         <v>58</v>
       </c>
-      <c t="s" s="3" r="B20">
+      <c r="C20" s="3" t="s">
         <v>59</v>
       </c>
-      <c t="s" s="3" r="C20">
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="21">
-      <c t="s" s="3" r="A21">
+      <c r="B21" s="3" t="s">
         <v>61</v>
       </c>
-      <c t="s" s="3" r="B21">
+      <c r="C21" s="3" t="s">
         <v>62</v>
       </c>
-      <c t="s" s="3" r="C21">
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="22">
-      <c t="s" s="3" r="A22">
+      <c r="B22" s="3" t="s">
         <v>64</v>
       </c>
-      <c t="s" s="3" r="B22">
+      <c r="C22" s="3" t="s">
         <v>65</v>
       </c>
-      <c t="s" s="3" r="C22">
+      <c r="D22" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="23">
-      <c t="s" s="3" r="A23">
+      <c r="B23" s="3" t="s">
         <v>67</v>
       </c>
-      <c t="s" s="3" r="B23">
+      <c r="C23" s="3" t="s">
         <v>68</v>
       </c>
-      <c t="s" s="3" r="C23">
+      <c r="D23" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="24">
-      <c t="s" s="3" r="A24">
+      <c r="B24" s="3" t="s">
         <v>70</v>
       </c>
-      <c t="s" s="3" r="B24">
+      <c r="C24" s="3" t="s">
         <v>71</v>
       </c>
-      <c t="s" s="3" r="C24">
+    </row>
+    <row r="25" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="25">
-      <c t="s" s="3" r="A25">
+      <c r="B25" s="3" t="s">
         <v>73</v>
       </c>
-      <c t="s" s="3" r="B25">
+      <c r="C25" s="3" t="s">
         <v>74</v>
       </c>
-      <c t="s" s="3" r="C25">
+    </row>
+    <row r="26" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="26">
-      <c t="s" s="3" r="A26">
+      <c r="B26" s="3" t="s">
         <v>76</v>
       </c>
-      <c t="s" s="3" r="B26">
+      <c r="C26" s="3" t="s">
         <v>77</v>
       </c>
-      <c t="s" s="3" r="C26">
+      <c r="D26" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="27">
-      <c t="s" s="3" r="A27">
+      <c r="B27" s="3" t="s">
         <v>79</v>
       </c>
-      <c t="s" s="3" r="B27">
+      <c r="C27" s="3" t="s">
         <v>80</v>
       </c>
-      <c t="s" s="3" r="C27">
+    </row>
+    <row r="28" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="28">
-      <c t="s" s="3" r="A28">
+      <c r="B28" s="3" t="s">
         <v>82</v>
       </c>
-      <c t="s" s="3" r="B28">
+      <c r="C28" s="3" t="s">
         <v>83</v>
       </c>
-      <c t="s" s="3" r="C28">
+      <c r="D28" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="29">
-      <c t="s" s="3" r="A29">
+      <c r="B29" s="3" t="s">
         <v>85</v>
       </c>
-      <c t="s" s="3" r="B29">
+    </row>
+    <row r="30" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="30">
-      <c t="s" s="3" r="A30">
+      <c r="B30" s="3" t="s">
         <v>87</v>
       </c>
-      <c t="s" s="3" r="B30">
+    </row>
+    <row r="31" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="31">
-      <c t="s" s="3" r="A31">
+      <c r="B31" s="3" t="s">
         <v>89</v>
       </c>
-      <c t="s" s="3" r="B31">
+    </row>
+    <row r="32" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="32">
-      <c t="s" s="3" r="A32">
+      <c r="B32" s="3" t="s">
         <v>91</v>
       </c>
-      <c t="s" s="3" r="B32">
+    </row>
+    <row r="33" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="33">
-      <c t="s" s="3" r="A33">
+      <c r="B33" s="3" t="s">
         <v>93</v>
       </c>
-      <c t="s" s="3" r="B33">
+    </row>
+    <row r="34" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="34">
-      <c t="s" s="3" r="A34">
+      <c r="B34" s="3" t="s">
         <v>95</v>
       </c>
-      <c t="s" s="3" r="B34">
+    </row>
+    <row r="35" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="35">
-      <c t="s" s="3" r="A35">
+      <c r="B35" s="3" t="s">
         <v>97</v>
       </c>
-      <c t="s" s="3" r="B35">
+    </row>
+    <row r="36" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="36">
-      <c t="s" s="3" r="A36">
+      <c r="B36" s="3" t="s">
         <v>99</v>
       </c>
-      <c t="s" s="3" r="B36">
+    </row>
+    <row r="37" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="37">
-      <c t="s" s="3" r="A37">
+      <c r="B37" s="3" t="s">
         <v>101</v>
       </c>
-      <c t="s" s="3" r="B37">
+    </row>
+    <row r="38" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="38">
-      <c t="s" s="3" r="A38">
+      <c r="B38" s="3" t="s">
         <v>103</v>
       </c>
-      <c t="s" s="3" r="B38">
+    </row>
+    <row r="39" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="39">
-      <c t="s" s="3" r="A39">
+      <c r="B39" s="3" t="s">
         <v>105</v>
       </c>
-      <c t="s" s="3" r="B39">
+    </row>
+    <row r="40" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="40">
-      <c t="s" s="3" r="A40">
+      <c r="B40" s="3" t="s">
         <v>107</v>
       </c>
-      <c t="s" s="3" r="B40">
+    </row>
+    <row r="41" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="41">
-      <c t="s" s="3" r="A41">
+      <c r="B41" s="3" t="s">
         <v>109</v>
       </c>
-      <c t="s" s="3" r="B41">
-        <v>110</v>
+    </row>
+    <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add integration tests for Next and NextStar
</commit_message>
<xml_diff>
--- a/Tests/CS3202 Test Cases.xlsx
+++ b/Tests/CS3202 Test Cases.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saima Mahmood\Documents\NUS\Sem 6\CS3201_CS3202 Software Engineering\cs3202 team 4 repo\Tests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="22400" windowHeight="15160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="121">
   <si>
     <t>Test Queries</t>
   </si>
@@ -273,9 +273,6 @@
     <t>Uses - Statement only</t>
   </si>
   <si>
-    <t>TestBasicModify_Query7</t>
-  </si>
-  <si>
     <t>Source7</t>
   </si>
   <si>
@@ -295,9 +292,6 @@
   </si>
   <si>
     <t>Source7</t>
-  </si>
-  <si>
-    <t>TestAffectsforProcedures_Query8</t>
   </si>
   <si>
     <t>Source8</t>
@@ -391,12 +385,21 @@
   <si>
     <t>Autotester Stops working</t>
   </si>
+  <si>
+    <t>TestBasicAffectsforProcedures_Query8</t>
+  </si>
+  <si>
+    <t>TestBasicAffectsStarforProcedures_Query8</t>
+  </si>
+  <si>
+    <t>TestBasicModifiesForStmt_Query7</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -421,6 +424,18 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -458,10 +473,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -470,8 +489,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -530,7 +554,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -565,7 +589,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -742,7 +766,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -750,21 +774,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="44.28515625" customWidth="1"/>
-    <col min="4" max="4" width="93.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" customWidth="1"/>
+    <col min="4" max="4" width="93.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -775,13 +799,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -792,7 +816,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -803,7 +827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -814,7 +838,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -825,7 +849,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
@@ -836,7 +860,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -847,7 +871,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
@@ -858,7 +882,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -869,7 +893,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -880,7 +904,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
@@ -891,7 +915,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
@@ -902,7 +926,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>36</v>
       </c>
@@ -913,7 +937,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>39</v>
       </c>
@@ -924,7 +948,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>42</v>
       </c>
@@ -935,7 +959,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
@@ -946,7 +970,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>48</v>
       </c>
@@ -957,7 +981,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>51</v>
       </c>
@@ -968,7 +992,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>54</v>
       </c>
@@ -979,7 +1003,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>57</v>
       </c>
@@ -990,7 +1014,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
         <v>60</v>
       </c>
@@ -1001,7 +1025,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>63</v>
       </c>
@@ -1012,13 +1036,13 @@
         <v>65</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>66</v>
       </c>
@@ -1029,13 +1053,13 @@
         <v>68</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="12">
       <c r="A24" s="3" t="s">
         <v>69</v>
       </c>
@@ -1046,7 +1070,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="12">
       <c r="A25" s="3" t="s">
         <v>72</v>
       </c>
@@ -1057,7 +1081,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="12">
       <c r="A26" s="3" t="s">
         <v>75</v>
       </c>
@@ -1068,10 +1092,10 @@
         <v>77</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="12">
       <c r="A27" s="3" t="s">
         <v>78</v>
       </c>
@@ -1082,7 +1106,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="12">
       <c r="A28" s="3" t="s">
         <v>81</v>
       </c>
@@ -1093,132 +1117,145 @@
         <v>83</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="12">
+      <c r="A29" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="D29" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="12">
+      <c r="A30" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="B30" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="12">
+      <c r="A31" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="12">
+      <c r="A32" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="12">
+      <c r="A33" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="12">
+      <c r="A34" s="8" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B32" s="3" t="s">
+      <c r="B34" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+    </row>
+    <row r="35" spans="1:2" ht="12">
+      <c r="A35" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+    <row r="36" spans="1:2" ht="12">
+      <c r="A36" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+    <row r="37" spans="1:2" ht="12">
+      <c r="A37" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+    <row r="38" spans="1:2" ht="12">
+      <c r="A38" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
+    <row r="39" spans="1:2" ht="12">
+      <c r="A39" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
+    <row r="40" spans="1:2" ht="12">
+      <c r="A40" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
+    <row r="41" spans="1:2" ht="12">
+      <c r="A41" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+    <row r="42" spans="1:2" ht="12">
+      <c r="A42" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>113</v>
+    <row r="47" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A47" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>